<commit_message>
update OV of 4th abd 5th week
</commit_message>
<xml_diff>
--- a/macros/APSAIA_VUV_2.xlsx
+++ b/macros/APSAIA_VUV_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="23">
   <si>
     <t>Run</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>SiPM289 SiPM290 SiPM377 SiPM378 XARAPUCA</t>
+  </si>
+  <si>
+    <t>4 4 4 4 2</t>
+  </si>
+  <si>
+    <t>4 4 4 4 2.5</t>
   </si>
   <si>
     <t>4 4 4 4 3</t>
@@ -487,7 +493,7 @@
     <col min="11" max="11" style="12" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -555,7 +561,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -588,7 +594,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -605,7 +611,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="5">
@@ -621,7 +627,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -638,7 +644,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="5">
@@ -654,7 +660,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -671,7 +677,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5">
@@ -687,7 +693,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -704,7 +710,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5">
@@ -720,7 +726,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -731,7 +737,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>14</v>
@@ -753,7 +759,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -764,13 +770,13 @@
         <v>12</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5">
@@ -786,7 +792,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -797,13 +803,13 @@
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5">
@@ -819,7 +825,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -830,13 +836,13 @@
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5">
@@ -852,7 +858,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -885,7 +891,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -918,7 +924,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -935,7 +941,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5">
@@ -951,7 +957,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -968,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
@@ -984,7 +990,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="5">
@@ -1017,7 +1023,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="5">
@@ -1050,7 +1056,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>14</v>
@@ -1083,7 +1089,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -1094,13 +1100,13 @@
         <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="5">
@@ -1116,7 +1122,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -1127,13 +1133,13 @@
         <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="5">
@@ -1149,7 +1155,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>14</v>
@@ -1182,7 +1188,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -1193,13 +1199,13 @@
         <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="5">
@@ -1215,7 +1221,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -1226,13 +1232,13 @@
         <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="5">
@@ -1248,7 +1254,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>14</v>
@@ -1281,7 +1287,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>14</v>
@@ -1314,7 +1320,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -1325,13 +1331,13 @@
         <v>12</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="5">
@@ -1347,7 +1353,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -1358,13 +1364,13 @@
         <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="5">
@@ -1380,7 +1386,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -1391,13 +1397,13 @@
         <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5">
@@ -1413,7 +1419,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -1424,13 +1430,13 @@
         <v>12</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5">
@@ -1446,7 +1452,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -1457,7 +1463,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>14</v>
@@ -1479,7 +1485,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -1490,13 +1496,13 @@
         <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5">
@@ -1512,7 +1518,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -1523,13 +1529,13 @@
         <v>12</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5">
@@ -1545,7 +1551,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -1556,13 +1562,13 @@
         <v>12</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5">
@@ -1578,7 +1584,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5">
@@ -1677,7 +1683,7 @@
         <v>25568.750520833335</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -1694,7 +1700,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5">
@@ -1727,7 +1733,7 @@
         <v>14</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5">
@@ -1760,7 +1766,7 @@
         <v>14</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="5">
@@ -1787,7 +1793,7 @@
         <v>12</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>14</v>
@@ -1820,7 +1826,7 @@
         <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>14</v>
@@ -1853,13 +1859,13 @@
         <v>12</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="5">
@@ -1886,13 +1892,13 @@
         <v>12</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="5">
@@ -1919,13 +1925,13 @@
         <v>12</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="5">
@@ -1952,13 +1958,13 @@
         <v>12</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="5">

</xml_diff>